<commit_message>
add LTW and GOV NRW 2022. also fix Zentrum partyfacts ID and MR Code switchup
</commit_message>
<xml_diff>
--- a/inst/extdata/Wahlleiter_Parteinamen.xlsx
+++ b/inst/extdata/Wahlleiter_Parteinamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Git_Projekte\bundeslaendeR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\bldrt\bundeslaendeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8135F2-69E4-41D1-9270-C976AE6A161B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E88166C-F4D0-47BF-86BF-492CA454BA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -5627,8 +5627,8 @@
   <dimension ref="A1:L510"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A490" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C513" sqref="C513"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G180" sqref="G180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41.7109375" defaultRowHeight="15"/>
@@ -7132,7 +7132,9 @@
       <c r="F51" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="G51" s="1"/>
+      <c r="G51" s="1">
+        <v>8993</v>
+      </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1" t="s">
@@ -10908,10 +10910,10 @@
         <v>1369</v>
       </c>
       <c r="G181">
+        <v>1798</v>
+      </c>
+      <c r="I181">
         <v>1</v>
-      </c>
-      <c r="I181">
-        <v>1798</v>
       </c>
       <c r="J181" t="s">
         <v>1384</v>

</xml_diff>